<commit_message>
presentazione e relazione ultimate e corrette
</commit_message>
<xml_diff>
--- a/Relazione/tempi_jetson.xlsx
+++ b/Relazione/tempi_jetson.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabri\Documents\Cuda Project\BirdEyeView\Relazione\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4F326E-AC95-4C48-86EB-BF396C181504}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B620080-DE59-49E6-A8FF-3A70BA9CA717}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D2F2C7F4-BC3F-47D8-A952-B5AF726D65BD}"/>
   </bookViews>
@@ -198,7 +198,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>Composizione tempo medio del frame </a:t>
+              <a:t>Composizione tempo medio analisi frame cuda  </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -514,7 +514,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="it-IT"/>
-              <a:t>Jetson - Tempi Esecuzione Medi Per Singolo Frame</a:t>
+              <a:t>Jetson - Tempi Esecuzione Medi Per Singolo Frame - CUDA</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -916,7 +916,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -1033,7 +1033,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
         <c:axId val="202889744"/>
         <c:axId val="258564000"/>
       </c:barChart>
@@ -1043,7 +1042,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1094,7 +1093,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -3768,15 +3767,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>119062</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4180,8 +4179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0ADE945-F4CE-403E-9A35-E75CAEBE8668}">
   <dimension ref="A1:Y1806"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R7" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="P10" workbookViewId="0">
+      <selection activeCell="AF19" sqref="AF19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>